<commit_message>
new aggregate with average distances
</commit_message>
<xml_diff>
--- a/aggregated_dataset.xlsx
+++ b/aggregated_dataset.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -451,6 +451,11 @@
           <t>Other</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>avg_distance_km</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
@@ -510,6 +515,9 @@
       <c r="Q2">
         <v>0</v>
       </c>
+      <c r="R2">
+        <v>4.136376498618044</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
@@ -569,6 +577,9 @@
       <c r="Q3">
         <v>1</v>
       </c>
+      <c r="R3">
+        <v>4.171829734708102</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
@@ -628,6 +639,9 @@
       <c r="Q4">
         <v>0</v>
       </c>
+      <c r="R4">
+        <v>4.490206231553414</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
@@ -687,6 +701,9 @@
       <c r="Q5">
         <v>1</v>
       </c>
+      <c r="R5">
+        <v>4.518039712920642</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
@@ -746,6 +763,9 @@
       <c r="Q6">
         <v>0</v>
       </c>
+      <c r="R6">
+        <v>4.508389709238768</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
@@ -805,6 +825,9 @@
       <c r="Q7">
         <v>6</v>
       </c>
+      <c r="R7">
+        <v>4.561800693261488</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
@@ -864,6 +887,9 @@
       <c r="Q8">
         <v>7</v>
       </c>
+      <c r="R8">
+        <v>4.723351366358533</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
@@ -923,6 +949,9 @@
       <c r="Q9">
         <v>10</v>
       </c>
+      <c r="R9">
+        <v>4.541151156676015</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
@@ -982,6 +1011,9 @@
       <c r="Q10">
         <v>2</v>
       </c>
+      <c r="R10">
+        <v>4.286881911154486</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
@@ -1041,6 +1073,9 @@
       <c r="Q11">
         <v>1</v>
       </c>
+      <c r="R11">
+        <v>4.675176933039502</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
@@ -1100,6 +1135,9 @@
       <c r="Q12">
         <v>0</v>
       </c>
+      <c r="R12">
+        <v>4.299951632670066</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
@@ -1159,6 +1197,9 @@
       <c r="Q13">
         <v>3</v>
       </c>
+      <c r="R13">
+        <v>3.709505535754547</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
@@ -1218,6 +1259,9 @@
       <c r="Q14">
         <v>1</v>
       </c>
+      <c r="R14">
+        <v>3.876734017006266</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
@@ -1277,6 +1321,9 @@
       <c r="Q15">
         <v>0</v>
       </c>
+      <c r="R15">
+        <v>4.476229029663664</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
@@ -1336,6 +1383,9 @@
       <c r="Q16">
         <v>0</v>
       </c>
+      <c r="R16">
+        <v>4.11879765724225</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
@@ -1395,6 +1445,9 @@
       <c r="Q17">
         <v>3</v>
       </c>
+      <c r="R17">
+        <v>4.385888662670677</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
@@ -1453,6 +1506,9 @@
       </c>
       <c r="Q18">
         <v>4</v>
+      </c>
+      <c r="R18">
+        <v>3.76326812791891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>